<commit_message>
Rectification de requet et de forme des nombres
</commit_message>
<xml_diff>
--- a/storage/26-04-2024/ENCAISSEMENT.xlsx
+++ b/storage/26-04-2024/ENCAISSEMENT.xlsx
@@ -71,11 +71,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -483,13 +485,13 @@
           <t>Chèques</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>725093.05</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>725093.05</v>
       </c>
     </row>
@@ -499,13 +501,13 @@
           <t>Coupon</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>21742.39</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>21742.39</v>
       </c>
     </row>
@@ -515,13 +517,13 @@
           <t>Espèces</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>219857.64</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>5262995.55</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>5262995.55</v>
       </c>
     </row>
@@ -531,13 +533,13 @@
           <t>Gratuit</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>106339.8</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>106339.8</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>106339.8</v>
       </c>
     </row>
@@ -547,13 +549,13 @@
           <t>Mvola</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>151987.06</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>151987.06</v>
       </c>
     </row>
@@ -563,29 +565,29 @@
           <t>TPE</t>
         </is>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>279654.34</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>279654.34</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="5" t="n">
         <v>326197.44</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="5" t="n">
         <v>6547812.19</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="5" t="n">
         <v>6547812.19</v>
       </c>
     </row>

</xml_diff>